<commit_message>
Class DIagram wass Added
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910D27AD-6C9C-4284-A4B2-9DDD619404AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4683D324-758F-45C8-91C2-87C0DFCCDA47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Antal Arbejds timer</t>
   </si>
   <si>
     <t>4 timer</t>
+  </si>
+  <si>
+    <t>4 timer 33 minutter</t>
   </si>
 </sst>
 </file>
@@ -391,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,8 +419,12 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="3">
+        <v>43980</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>

</xml_diff>

<commit_message>
models on the clien side has been made. as well as references from top layer to repositorys
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4683D324-758F-45C8-91C2-87C0DFCCDA47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FC0C93-A0C9-4B62-8700-F0F99841E4D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -395,7 +395,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +427,9 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
+      <c r="A4" s="3">
+        <v>43982</v>
+      </c>
       <c r="B4" s="5"/>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Setting up a basic idea for the UI Layout
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FC0C93-A0C9-4B62-8700-F0F99841E4D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822F3E76-DAF4-4529-9F62-83FAEA78375C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Antal Arbejds timer</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>4 timer 33 minutter</t>
+  </si>
+  <si>
+    <t>2 timer 30 minutter</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +433,9 @@
       <c r="A4" s="3">
         <v>43982</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>

</xml_diff>

<commit_message>
Startet working on Singelplayer game logic
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822F3E76-DAF4-4529-9F62-83FAEA78375C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A212912-5CC9-43A8-9609-DA58300C1F43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,7 +398,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +438,9 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
+      <c r="A5" s="3">
+        <v>43983</v>
+      </c>
       <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Working on the comunication between TTT_Repository and WPF MainWindow
Still working on the Singelplayer functionalety
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57370F1F-D634-43DB-84B2-372F174EA81C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D56F0D3-8B84-4691-BE62-92714FC0E6BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Antal Arbejds timer</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>2 timer 30 minutter</t>
+  </si>
+  <si>
+    <t>6 timer</t>
   </si>
 </sst>
 </file>
@@ -397,7 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -441,7 +444,9 @@
       <c r="A5" s="3">
         <v>43983</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>

</xml_diff>

<commit_message>
Update to the Documentasion and work hours spetsheet
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D56F0D3-8B84-4691-BE62-92714FC0E6BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B449DEF4-302D-4A10-8FC3-1FD1A657F881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,19 +27,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Antal Arbejds timer</t>
+    <t>Amount of work hours</t>
   </si>
   <si>
-    <t>4 timer</t>
+    <t>4 hours</t>
   </si>
   <si>
-    <t>4 timer 33 minutter</t>
+    <t>7 hours 30 minuts</t>
   </si>
   <si>
-    <t>2 timer 30 minutter</t>
+    <t>2 hours 30 minuts</t>
   </si>
   <si>
-    <t>6 timer</t>
+    <t>4 hours 33 minuts</t>
   </si>
 </sst>
 </file>
@@ -400,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +429,7 @@
         <v>43980</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -445,7 +445,7 @@
         <v>43983</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Big change to the WPF layout style
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kasp837c\source\repos\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B449DEF4-302D-4A10-8FC3-1FD1A657F881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28922" yWindow="-122" windowWidth="29045" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Amount of work hours</t>
   </si>
@@ -40,12 +39,15 @@
   </si>
   <si>
     <t>4 hours 33 minuts</t>
+  </si>
+  <si>
+    <t>8 hours 30 minuts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -397,26 +399,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>43979</v>
       </c>
@@ -424,7 +426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>43980</v>
       </c>
@@ -432,7 +434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>43982</v>
       </c>
@@ -440,7 +442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>43983</v>
       </c>
@@ -448,35 +450,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>43984</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
     </row>

</xml_diff>

<commit_message>
New multiWindow application made. Singelplayer and Multiplayer is now on two seperate windows
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kasp837c\source\repos\Tic-Tac-Toe\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089DB292-FF62-4A53-BFE6-DF4349DB94AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28922" yWindow="-122" windowWidth="29045" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,26 +400,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="27.25" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>43979</v>
       </c>
@@ -426,7 +427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>43980</v>
       </c>
@@ -434,7 +435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>43982</v>
       </c>
@@ -442,7 +443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>43983</v>
       </c>
@@ -450,7 +451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>43984</v>
       </c>
@@ -458,31 +459,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update to the documentasion  Word and lsx got updatet
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089DB292-FF62-4A53-BFE6-DF4349DB94AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4DB35B-2215-4D3A-934D-17726F2E804E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,16 +34,16 @@
     <t>4 hours</t>
   </si>
   <si>
-    <t>7 hours 30 minuts</t>
-  </si>
-  <si>
-    <t>2 hours 30 minuts</t>
-  </si>
-  <si>
-    <t>4 hours 33 minuts</t>
-  </si>
-  <si>
-    <t>8 hours 30 minuts</t>
+    <t>14 hours 30 minutes</t>
+  </si>
+  <si>
+    <t>7 hours 30 minutes</t>
+  </si>
+  <si>
+    <t>2 hours 30 minutes</t>
+  </si>
+  <si>
+    <t>4 hours 33 minutes</t>
   </si>
 </sst>
 </file>
@@ -404,7 +405,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +433,7 @@
         <v>43980</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -440,7 +441,7 @@
         <v>43982</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -448,7 +449,7 @@
         <v>43983</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -456,7 +457,7 @@
         <v>43984</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update to the documentasion
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kasp837c\source\repos\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4DB35B-2215-4D3A-934D-17726F2E804E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28922" yWindow="-122" windowWidth="29045" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Amount of work hours</t>
   </si>
@@ -44,12 +42,18 @@
   </si>
   <si>
     <t>4 hours 33 minutes</t>
+  </si>
+  <si>
+    <t>6 hours 24 minutes</t>
+  </si>
+  <si>
+    <t>TOTAL:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,26 +405,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>43979</v>
       </c>
@@ -428,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>43980</v>
       </c>
@@ -436,7 +440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>43982</v>
       </c>
@@ -444,7 +448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>43983</v>
       </c>
@@ -452,7 +456,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>43984</v>
       </c>
@@ -460,32 +464,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>43985</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="19.05" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="19.05" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="19.05" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="19.05" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="19.05" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+    <row r="13" spans="1:2" ht="19.05" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="B13" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the documentasion and startet practesing making a web socet via console applications • ServerTeste • ConectionTester
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kasp837c\source\repos\Tic-Tac-Toe\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75C1B2E-716B-40C4-8E88-164F93D9D51D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28922" yWindow="-122" windowWidth="29045" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,16 +45,16 @@
     <t>4 hours 33 minutes</t>
   </si>
   <si>
-    <t>6 hours 24 minutes</t>
-  </si>
-  <si>
     <t>TOTAL:</t>
+  </si>
+  <si>
+    <t>7 hours 24 minutes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,26 +406,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="27.25" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>43979</v>
       </c>
@@ -432,7 +433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>43980</v>
       </c>
@@ -440,7 +441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>43982</v>
       </c>
@@ -448,7 +449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>43983</v>
       </c>
@@ -456,7 +457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>43984</v>
       </c>
@@ -464,37 +465,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>43985</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="19.05" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2" ht="19.05" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" ht="19.05" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" ht="19.05" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" ht="19.05" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" ht="19.05" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="5"/>
     </row>

</xml_diff>

<commit_message>
Building and testing a test server and client for websocets
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kasp837c\source\repos\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75C1B2E-716B-40C4-8E88-164F93D9D51D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28922" yWindow="-122" windowWidth="29045" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -406,26 +405,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>43979</v>
       </c>
@@ -433,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>43980</v>
       </c>
@@ -441,7 +440,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>43982</v>
       </c>
@@ -449,7 +448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>43983</v>
       </c>
@@ -457,7 +456,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>43984</v>
       </c>
@@ -465,7 +464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>43985</v>
       </c>
@@ -473,27 +472,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
+    <row r="8" spans="1:2" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>43986</v>
+      </c>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
successfull test enviorment for a singel connection
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kasp837c\source\repos\Tic-Tac-Toe\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B4538B-EAD8-4320-935D-7CDF44F359AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28922" yWindow="-122" windowWidth="29045" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Amount of work hours</t>
   </si>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,26 +406,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="27.25" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>43979</v>
       </c>
@@ -432,7 +433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>43980</v>
       </c>
@@ -440,7 +441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>43982</v>
       </c>
@@ -448,7 +449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>43983</v>
       </c>
@@ -456,7 +457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>43984</v>
       </c>
@@ -464,7 +465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>43985</v>
       </c>
@@ -472,29 +473,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>43986</v>
       </c>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:2" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Working on the WebSocket server. for the multiplayer game mode
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B4538B-EAD8-4320-935D-7CDF44F359AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA9103A-D9C7-4492-85DA-80AB91973D3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Amount of work hours</t>
   </si>
@@ -49,13 +49,19 @@
   </si>
   <si>
     <t>7 hours 24 minutes</t>
+  </si>
+  <si>
+    <t>Time above is time spend on the project + study time</t>
+  </si>
+  <si>
+    <t>7 hours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +87,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -112,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -127,6 +140,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,35 +487,46 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>43986</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>43987</v>
+      </c>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" ht="19.149999999999999" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="5"/>
+    </row>
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Creating the Multiplayer client UI
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2389694-1B08-4686-B186-EC2F12BA94E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4A11B9-1398-403F-A54B-F120C5835C1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Amount of work hours</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>7 hours</t>
+  </si>
+  <si>
+    <t>startet kl 9:45</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,10 +502,14 @@
       <c r="A9" s="3">
         <v>43987</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
+      <c r="A10" s="3">
+        <v>43988</v>
+      </c>
       <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
End of the day commit. Stil working on the WebSokets server
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B5FF5D-A177-4F8E-98A2-32CD770F80F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B74F960-BCA4-423B-9518-16580B8C4FAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
     <t>7 hours</t>
   </si>
   <si>
-    <t>startet kl 9:45 | pause fra 19:00 -</t>
+    <t>13 Hours 25 Minutes</t>
   </si>
 </sst>
 </file>
@@ -128,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -144,9 +144,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +427,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +502,7 @@
       <c r="A9" s="3">
         <v>43987</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Server and Client upgrade
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B74F960-BCA4-423B-9518-16580B8C4FAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AC6A17-A719-4155-9676-B1DB40C03C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Amount of work hours</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>13 Hours 25 Minutes</t>
+  </si>
+  <si>
+    <t>11 Hours 38 Minutes</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,10 +513,14 @@
       <c r="A10" s="3">
         <v>43988</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="3">
+        <v>43989</v>
+      </c>
       <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Client sidte class diagram has been updatet. and old ons has been deletet
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37AC6A17-A719-4155-9676-B1DB40C03C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEBC415-A2AB-4B3A-86FF-F91AE1B41373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
     <t>13 Hours 25 Minutes</t>
   </si>
   <si>
-    <t>11 Hours 38 Minutes</t>
+    <t>13 Hours 8 Minutes</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Big update to all Diagrams
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEBC415-A2AB-4B3A-86FF-F91AE1B41373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D80C7FB-C22F-4B56-A521-5E93EC51C08D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Amount of work hours</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>13 Hours 8 Minutes</t>
+  </si>
+  <si>
+    <t>Startet kl. 12:00</t>
+  </si>
+  <si>
+    <t>74 hours</t>
   </si>
 </sst>
 </file>
@@ -430,7 +436,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +527,9 @@
       <c r="A11" s="3">
         <v>43989</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
@@ -531,7 +539,9 @@
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">

</xml_diff>

<commit_message>
Update to the documentasion paipers
</commit_message>
<xml_diff>
--- a/Documentation/Work Time Table.xlsx
+++ b/Documentation/Work Time Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjran\source\repos\Visual Studio\Tic-Tac-Toe\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D80C7FB-C22F-4B56-A521-5E93EC51C08D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B26E12-8CC3-440F-9177-851752DFFB65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,10 +63,10 @@
     <t>13 Hours 8 Minutes</t>
   </si>
   <si>
-    <t>Startet kl. 12:00</t>
-  </si>
-  <si>
-    <t>74 hours</t>
+    <t>12 Hours</t>
+  </si>
+  <si>
+    <t>Started at 00:00</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,16 +532,18 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="3">
+        <v>43990</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="B13" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">

</xml_diff>